<commit_message>
fixed validate method from (OCABUNDLE class).
</commit_message>
<xml_diff>
--- a/tests/datasets/data_entry.xlsx
+++ b/tests/datasets/data_entry.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068DDBCA-986D-3E40-B7CF-4379EF9DFA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD869111-ABB6-034A-AAE3-E17021C60B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -233,13 +233,13 @@
     <t>S</t>
   </si>
   <si>
-    <t>age</t>
-  </si>
-  <si>
     <t>sugar</t>
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>aage</t>
   </si>
 </sst>
 </file>
@@ -1264,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B2">
         <f>IF(ISBLANK('Data Entry'!$B$2), "", 'Data Entry'!$B$2)</f>
@@ -1402,7 +1402,7 @@
         <v>123456789</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5">
         <f>IF(ISBLANK('Data Entry'!$F$5), "", 'Data Entry'!$F$5)</f>
@@ -1423,7 +1423,7 @@
         <v>123456789</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6">
         <f>IF(ISBLANK('Data Entry'!$D$6), "", 'Data Entry'!$D$6)</f>

</xml_diff>

<commit_message>
updates on reading xls files and fixed entry codes.
</commit_message>
<xml_diff>
--- a/tests/datasets/data_entry.xlsx
+++ b/tests/datasets/data_entry.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD869111-ABB6-034A-AAE3-E17021C60B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EF2DF9-A262-D444-B096-C939EF9CF91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema Description" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
   <si>
     <t>This is an Excel workbook for data entry.</t>
   </si>
@@ -231,12 +231,6 @@
   </si>
   <si>
     <t>S</t>
-  </si>
-  <si>
-    <t>sugar</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
   <si>
     <t>aage</t>
@@ -1265,7 +1259,7 @@
   <dimension ref="A1:G1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1298,7 +1292,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <f>IF(ISBLANK('Data Entry'!$B$2), "", 'Data Entry'!$B$2)</f>
@@ -1401,8 +1395,9 @@
         <f>IF(ISBLANK('Data Entry'!$D$5), "", 'Data Entry'!$D$5)</f>
         <v>123456789</v>
       </c>
-      <c r="E5" t="s">
-        <v>67</v>
+      <c r="E5">
+        <f>IF(ISBLANK('Data Entry'!$E$4), "", 'Data Entry'!$E$4)</f>
+        <v>234516789</v>
       </c>
       <c r="F5">
         <f>IF(ISBLANK('Data Entry'!$F$5), "", 'Data Entry'!$F$5)</f>
@@ -1423,7 +1418,7 @@
         <v>123456789</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <f>IF(ISBLANK('Data Entry'!$D$6), "", 'Data Entry'!$D$6)</f>

</xml_diff>

<commit_message>
adding an error collection object.
</commit_message>
<xml_diff>
--- a/tests/datasets/data_entry.xlsx
+++ b/tests/datasets/data_entry.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EF2DF9-A262-D444-B096-C939EF9CF91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801146B5-A2BA-184D-AB9C-0580C0900EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema Description" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
   <si>
     <t>This is an Excel workbook for data entry.</t>
   </si>
@@ -233,7 +233,7 @@
     <t>S</t>
   </si>
   <si>
-    <t>aage</t>
+    <t>mmm</t>
   </si>
 </sst>
 </file>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1259,7 +1259,7 @@
   <dimension ref="A1:G1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1291,16 +1291,6 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2">
-        <f>IF(ISBLANK('Data Entry'!$B$2), "", 'Data Entry'!$B$2)</f>
-        <v>123456789</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
       <c r="D2">
         <f>IF(ISBLANK('Data Entry'!$D$2), "", 'Data Entry'!$D$2)</f>
         <v>123456789</v>
@@ -1309,27 +1299,14 @@
         <f>IF(ISBLANK('Data Entry'!$E$2), "", 'Data Entry'!$E$2)</f>
         <v>234516789</v>
       </c>
-      <c r="F2">
-        <f>IF(ISBLANK('Data Entry'!$F$2), "", 'Data Entry'!$F$2)</f>
-        <v>234516789</v>
-      </c>
       <c r="G2">
         <f>IF(ISBLANK('Data Entry'!$G$2), "", 'Data Entry'!$G$2)</f>
         <v>234516789</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <f>IF(ISBLANK('Data Entry'!$A$3), "", 'Data Entry'!$A$3)</f>
-        <v>150</v>
-      </c>
-      <c r="B3">
-        <f>IF(ISBLANK('Data Entry'!$B$3), "", 'Data Entry'!$B$3)</f>
-        <v>123456789</v>
-      </c>
-      <c r="C3" t="str">
-        <f>IF(ISBLANK('Data Entry'!$C$3), "", VLOOKUP('Data Entry'!$C$3, 'Schema Description'!$A$40:$B$41, 2))</f>
-        <v>S</v>
+      <c r="C3" t="s">
+        <v>67</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK('Data Entry'!$D$3), "", 'Data Entry'!$D$3)</f>
@@ -1353,14 +1330,6 @@
         <f>IF(ISBLANK('Data Entry'!$A$4), "", 'Data Entry'!$A$4)</f>
         <v>230</v>
       </c>
-      <c r="B4">
-        <f>IF(ISBLANK('Data Entry'!$B$4), "", 'Data Entry'!$B$4)</f>
-        <v>123456789</v>
-      </c>
-      <c r="C4" t="str">
-        <f>IF(ISBLANK('Data Entry'!$C$4), "", VLOOKUP('Data Entry'!$C$4, 'Schema Description'!$A$40:$B$41, 2))</f>
-        <v>S</v>
-      </c>
       <c r="D4">
         <f>IF(ISBLANK('Data Entry'!$D$4), "", 'Data Entry'!$D$4)</f>
         <v>123456789</v>
@@ -1383,14 +1352,6 @@
         <f>IF(ISBLANK('Data Entry'!$A$5), "", 'Data Entry'!$A$5)</f>
         <v>130</v>
       </c>
-      <c r="B5">
-        <f>IF(ISBLANK('Data Entry'!$B$5), "", 'Data Entry'!$B$5)</f>
-        <v>123456789</v>
-      </c>
-      <c r="C5" t="str">
-        <f>IF(ISBLANK('Data Entry'!$C$5), "", VLOOKUP('Data Entry'!$C$5, 'Schema Description'!$A$40:$B$41, 2))</f>
-        <v>B</v>
-      </c>
       <c r="D5">
         <f>IF(ISBLANK('Data Entry'!$D$5), "", 'Data Entry'!$D$5)</f>
         <v>123456789</v>
@@ -1413,12 +1374,8 @@
         <f>IF(ISBLANK('Data Entry'!$A$6), "", 'Data Entry'!$A$6)</f>
         <v>211</v>
       </c>
-      <c r="B6">
-        <f>IF(ISBLANK('Data Entry'!$B$6), "", 'Data Entry'!$B$6)</f>
-        <v>123456789</v>
-      </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D6">
         <f>IF(ISBLANK('Data Entry'!$D$6), "", 'Data Entry'!$D$6)</f>

</xml_diff>

<commit_message>
merge: Err collection branch (#1)
* validation rules.

* validate function.

* fixed validate method from (OCABUNDLE class).

* fixed validate method from (OCABUNDLE class).

* updates on reading xls files and fixed entry codes.

* eslint (lib and tests).

* adding an error collection object.

* datasets: accepting CSV.

---------

Co-authored-by: Steven-Mugisha <smugisha@uoguelph.ca>
</commit_message>
<xml_diff>
--- a/tests/datasets/data_entry.xlsx
+++ b/tests/datasets/data_entry.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4411DEC4-7EE0-B544-BB8B-2C60F8DF28E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801146B5-A2BA-184D-AB9C-0580C0900EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
   <si>
     <t>This is an Excel workbook for data entry.</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>mmm</t>
   </si>
 </sst>
 </file>
@@ -695,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1255,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1288,18 +1291,6 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <f>IF(ISBLANK('Data Entry'!$A$2), "", 'Data Entry'!$A$2)</f>
-        <v>120</v>
-      </c>
-      <c r="B2">
-        <f>IF(ISBLANK('Data Entry'!$B$2), "", 'Data Entry'!$B$2)</f>
-        <v>123456789</v>
-      </c>
-      <c r="C2" t="str">
-        <f>IF(ISBLANK('Data Entry'!$C$2), "", VLOOKUP('Data Entry'!$C$2, 'Schema Description'!$A$40:$B$41, 2))</f>
-        <v>B</v>
-      </c>
       <c r="D2">
         <f>IF(ISBLANK('Data Entry'!$D$2), "", 'Data Entry'!$D$2)</f>
         <v>123456789</v>
@@ -1308,27 +1299,14 @@
         <f>IF(ISBLANK('Data Entry'!$E$2), "", 'Data Entry'!$E$2)</f>
         <v>234516789</v>
       </c>
-      <c r="F2">
-        <f>IF(ISBLANK('Data Entry'!$F$2), "", 'Data Entry'!$F$2)</f>
-        <v>234516789</v>
-      </c>
       <c r="G2">
         <f>IF(ISBLANK('Data Entry'!$G$2), "", 'Data Entry'!$G$2)</f>
         <v>234516789</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <f>IF(ISBLANK('Data Entry'!$A$3), "", 'Data Entry'!$A$3)</f>
-        <v>150</v>
-      </c>
-      <c r="B3">
-        <f>IF(ISBLANK('Data Entry'!$B$3), "", 'Data Entry'!$B$3)</f>
-        <v>123456789</v>
-      </c>
-      <c r="C3" t="str">
-        <f>IF(ISBLANK('Data Entry'!$C$3), "", VLOOKUP('Data Entry'!$C$3, 'Schema Description'!$A$40:$B$41, 2))</f>
-        <v>S</v>
+      <c r="C3" t="s">
+        <v>67</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK('Data Entry'!$D$3), "", 'Data Entry'!$D$3)</f>
@@ -1352,14 +1330,6 @@
         <f>IF(ISBLANK('Data Entry'!$A$4), "", 'Data Entry'!$A$4)</f>
         <v>230</v>
       </c>
-      <c r="B4">
-        <f>IF(ISBLANK('Data Entry'!$B$4), "", 'Data Entry'!$B$4)</f>
-        <v>123456789</v>
-      </c>
-      <c r="C4" t="str">
-        <f>IF(ISBLANK('Data Entry'!$C$4), "", VLOOKUP('Data Entry'!$C$4, 'Schema Description'!$A$40:$B$41, 2))</f>
-        <v>S</v>
-      </c>
       <c r="D4">
         <f>IF(ISBLANK('Data Entry'!$D$4), "", 'Data Entry'!$D$4)</f>
         <v>123456789</v>
@@ -1382,20 +1352,12 @@
         <f>IF(ISBLANK('Data Entry'!$A$5), "", 'Data Entry'!$A$5)</f>
         <v>130</v>
       </c>
-      <c r="B5">
-        <f>IF(ISBLANK('Data Entry'!$B$5), "", 'Data Entry'!$B$5)</f>
-        <v>123456789</v>
-      </c>
-      <c r="C5" t="str">
-        <f>IF(ISBLANK('Data Entry'!$C$5), "", VLOOKUP('Data Entry'!$C$5, 'Schema Description'!$A$40:$B$41, 2))</f>
-        <v>B</v>
-      </c>
       <c r="D5">
         <f>IF(ISBLANK('Data Entry'!$D$5), "", 'Data Entry'!$D$5)</f>
         <v>123456789</v>
       </c>
       <c r="E5">
-        <f>IF(ISBLANK('Data Entry'!$E$5), "", 'Data Entry'!$E$5)</f>
+        <f>IF(ISBLANK('Data Entry'!$E$4), "", 'Data Entry'!$E$4)</f>
         <v>234516789</v>
       </c>
       <c r="F5">
@@ -1412,13 +1374,8 @@
         <f>IF(ISBLANK('Data Entry'!$A$6), "", 'Data Entry'!$A$6)</f>
         <v>211</v>
       </c>
-      <c r="B6">
-        <f>IF(ISBLANK('Data Entry'!$B$6), "", 'Data Entry'!$B$6)</f>
-        <v>123456789</v>
-      </c>
-      <c r="C6" t="str">
-        <f>IF(ISBLANK('Data Entry'!$C$6), "", VLOOKUP('Data Entry'!$C$6, 'Schema Description'!$A$40:$B$41, 2))</f>
-        <v>B</v>
+      <c r="C6" t="s">
+        <v>66</v>
       </c>
       <c r="D6">
         <f>IF(ISBLANK('Data Entry'!$D$6), "", 'Data Entry'!$D$6)</f>
@@ -1665,7 +1622,7 @@
         <v/>
       </c>
       <c r="E14" t="str">
-        <f>IF(ISBLANK('Data Entry'!$E$14), "", 'Data Entry'!$E$14)</f>
+        <f>IF(ISBLANK('Data Entry'!$E$13), "", 'Data Entry'!$E$13)</f>
         <v/>
       </c>
       <c r="F14" t="str">

</xml_diff>

<commit_message>
attribute format errors fix.
</commit_message>
<xml_diff>
--- a/tests/datasets/data_entry.xlsx
+++ b/tests/datasets/data_entry.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801146B5-A2BA-184D-AB9C-0580C0900EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D71E1C4-8952-4342-8A13-ED6A6105F2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema Description" sheetId="1" r:id="rId1"/>
     <sheet name="Data Entry" sheetId="2" r:id="rId2"/>
-    <sheet name="Schema conformant data" sheetId="3" r:id="rId3"/>
+    <sheet name="Schema Conformant Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1259,7 +1259,7 @@
   <dimension ref="A1:G1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1643,10 +1643,6 @@
         <f>IF(ISBLANK('Data Entry'!$B$15), "", 'Data Entry'!$B$15)</f>
         <v/>
       </c>
-      <c r="C15" t="str">
-        <f>IF(ISBLANK('Data Entry'!$C$15), "", VLOOKUP('Data Entry'!$C$15, 'Schema Description'!$A$40:$B$41, 2))</f>
-        <v/>
-      </c>
       <c r="D15" t="str">
         <f>IF(ISBLANK('Data Entry'!$D$15), "", 'Data Entry'!$D$15)</f>
         <v/>

</xml_diff>

<commit_message>
datetime & numeric fixes (#2)
* conformance check fix.

* attribute format errors fix.

* adding support for zip bundles.

* array type fix

* Boolean type check fix.

* entrycodes  error-checks.

* character encoding.

* numeric and datetime checks.
</commit_message>
<xml_diff>
--- a/tests/datasets/data_entry.xlsx
+++ b/tests/datasets/data_entry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801146B5-A2BA-184D-AB9C-0580C0900EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C38CCBD-1997-3147-8B04-E6A072455B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema Description" sheetId="1" r:id="rId1"/>
     <sheet name="Data Entry" sheetId="2" r:id="rId2"/>
-    <sheet name="Schema conformant data" sheetId="3" r:id="rId3"/>
+    <sheet name="Schema Conformant Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
   <si>
     <t>This is an Excel workbook for data entry.</t>
   </si>
@@ -233,7 +233,10 @@
     <t>S</t>
   </si>
   <si>
-    <t>mmm</t>
+    <t>\xf1\x28\x80\x28</t>
+  </si>
+  <si>
+    <t>mm</t>
   </si>
 </sst>
 </file>
@@ -1259,12 +1262,15 @@
   <dimension ref="A1:G1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="15" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1291,6 +1297,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
       <c r="D2">
         <f>IF(ISBLANK('Data Entry'!$D$2), "", 'Data Entry'!$D$2)</f>
         <v>123456789</v>
@@ -1299,15 +1311,16 @@
         <f>IF(ISBLANK('Data Entry'!$E$2), "", 'Data Entry'!$E$2)</f>
         <v>234516789</v>
       </c>
+      <c r="F2">
+        <f>IF(ISBLANK('Data Entry'!$F$3), "", 'Data Entry'!$F$3)</f>
+        <v>234516789</v>
+      </c>
       <c r="G2">
         <f>IF(ISBLANK('Data Entry'!$G$2), "", 'Data Entry'!$G$2)</f>
         <v>234516789</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
       <c r="D3">
         <f>IF(ISBLANK('Data Entry'!$D$3), "", 'Data Entry'!$D$3)</f>
         <v>123456789</v>
@@ -1641,10 +1654,6 @@
       </c>
       <c r="B15" t="str">
         <f>IF(ISBLANK('Data Entry'!$B$15), "", 'Data Entry'!$B$15)</f>
-        <v/>
-      </c>
-      <c r="C15" t="str">
-        <f>IF(ISBLANK('Data Entry'!$C$15), "", VLOOKUP('Data Entry'!$C$15, 'Schema Description'!$A$40:$B$41, 2))</f>
         <v/>
       </c>
       <c r="D15" t="str">

</xml_diff>